<commit_message>
Wrong shortest path highlighted
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8120" yWindow="0" windowWidth="17480" windowHeight="14420" tabRatio="500"/>
+    <workbookView xWindow="11000" yWindow="0" windowWidth="25600" windowHeight="14420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -713,7 +713,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -842,7 +842,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>2374</v>
+        <v>2734</v>
       </c>
     </row>
     <row r="6" spans="1:7">

</xml_diff>